<commit_message>
Added stream while extracting pdf and sropping all the columns that are empty and duplicates
</commit_message>
<xml_diff>
--- a/modified_tables/table_10.xlsx
+++ b/modified_tables/table_10.xlsx
@@ -14,33 +14,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>2,082</t>
-  </si>
-  <si>
-    <t>494</t>
-  </si>
-  <si>
-    <t>351</t>
-  </si>
-  <si>
-    <t>169</t>
-  </si>
-  <si>
-    <t>447</t>
-  </si>
-  <si>
-    <t>1,153</t>
-  </si>
-  <si>
-    <t>3,920</t>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>Electricity consumption</t>
+  </si>
+  <si>
+    <t>Total electricity consumption</t>
+  </si>
+  <si>
+    <t>33,104,461</t>
+  </si>
+  <si>
+    <t>33,035,150</t>
+  </si>
+  <si>
+    <t>32,208,132</t>
+  </si>
+  <si>
+    <t>of which green electricity</t>
+  </si>
+  <si>
+    <t>32,782,553</t>
+  </si>
+  <si>
+    <t>33,005,705</t>
+  </si>
+  <si>
+    <t>32,036,926</t>
+  </si>
+  <si>
+    <t>Individual electricity consumption (kWh per FTE)</t>
+  </si>
+  <si>
+    <t>7,116</t>
+  </si>
+  <si>
+    <t>7,000</t>
+  </si>
+  <si>
+    <t>6,734</t>
+  </si>
+  <si>
+    <t>District heating consumption</t>
+  </si>
+  <si>
+    <t>Total district heating consumption</t>
+  </si>
+  <si>
+    <t>18,964,126</t>
+  </si>
+  <si>
+    <t>18,124,104</t>
+  </si>
+  <si>
+    <t>18,563,309</t>
+  </si>
+  <si>
+    <t>Individual heating consumption (kWh per FTE)</t>
+  </si>
+  <si>
+    <t>4,077</t>
+  </si>
+  <si>
+    <t>3,841</t>
+  </si>
+  <si>
+    <t>3,881</t>
   </si>
 </sst>
 </file>
@@ -398,50 +449,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>